<commit_message>
Updated 'cell_culture_samples.xlsx' in the `TEST/RawData/StandardCurve` directory
</commit_message>
<xml_diff>
--- a/qPCR_READER/TEST/RawData/StandardCurve/cell_culture_samples.xlsx
+++ b/qPCR_READER/TEST/RawData/StandardCurve/cell_culture_samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardharris/PycharmProjects/TIBD_biochem/qPCR_READER/TEST/RawData/StandardCurve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E658174-2569-B044-BF41-2A5E0FD99ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D6F690-2EEF-B948-99A8-32CA20319B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{36D3BA4A-0F62-4F4D-A8E6-FD26F3E052DF}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="35840" windowHeight="20380" xr2:uid="{36D3BA4A-0F62-4F4D-A8E6-FD26F3E052DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>cDNA_ug</t>
-  </si>
-  <si>
     <t>Water_uL</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>HH</t>
+  </si>
+  <si>
+    <t>cDNA_ng</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,10 +502,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -513,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="2">
         <v>16</v>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="2">
         <v>32</v>
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="2">
         <v>96</v>
@@ -546,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C5" s="2">
         <v>288</v>
@@ -557,7 +557,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C6" s="2">
         <v>864</v>
@@ -568,7 +568,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C7" s="2">
         <v>2592</v>
@@ -579,7 +579,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C8" s="2">
         <v>7776.0000000000009</v>
@@ -590,7 +590,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C9" s="2">
         <v>23328</v>
@@ -598,10 +598,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C10" s="2">
         <v>8</v>
@@ -609,10 +609,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C11" s="2">
         <v>16</v>
@@ -620,10 +620,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C12" s="2">
         <v>48</v>
@@ -631,10 +631,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C13" s="2">
         <v>144</v>
@@ -642,10 +642,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C14" s="2">
         <v>432</v>
@@ -653,10 +653,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C15" s="2">
         <v>1296</v>
@@ -664,10 +664,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C16" s="2">
         <v>3888.0000000000005</v>
@@ -675,10 +675,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C17" s="2">
         <v>11664</v>

</xml_diff>